<commit_message>
Movido callbacks opengl para jogo
</commit_message>
<xml_diff>
--- a/me264.xlsx
+++ b/me264.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\Visual Studio 2013\Projects\CG-Tp1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEFET\8o Periodo\Computacao Grafica\CG-Tp1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -199,9 +199,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -239,7 +239,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -311,7 +311,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="U40" sqref="U40:V41"/>
+    <sheetView tabSelected="1" topLeftCell="F55" workbookViewId="0">
+      <selection activeCell="K66" sqref="K66:K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F2">
         <v>6.2</v>
@@ -520,7 +520,7 @@
       </c>
       <c r="P2">
         <f t="shared" si="0"/>
-        <v>0.1059322033898305</v>
+        <v>9.3220338983050849E-2</v>
       </c>
       <c r="Q2">
         <f t="shared" si="0"/>
@@ -543,7 +543,7 @@
         <v>4.5</v>
       </c>
       <c r="E3">
-        <v>2.8</v>
+        <v>2.5</v>
       </c>
       <c r="F3">
         <v>6.2</v>
@@ -564,7 +564,7 @@
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P37" si="3">E3/23.6</f>
-        <v>0.11864406779661016</v>
+        <v>0.1059322033898305</v>
       </c>
       <c r="Q3">
         <f t="shared" ref="Q3:Q37" si="4">F3/23.6</f>
@@ -654,7 +654,7 @@
         <v>-1</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6">
         <v>6.2</v>
@@ -672,7 +672,7 @@
       </c>
       <c r="P6">
         <f t="shared" si="3"/>
-        <v>0.1271186440677966</v>
+        <v>8.4745762711864403E-2</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
@@ -695,7 +695,7 @@
         <v>-2.2000000000000002</v>
       </c>
       <c r="E7">
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="F7">
         <v>6.2</v>
@@ -719,7 +719,7 @@
       </c>
       <c r="P7">
         <f t="shared" si="3"/>
-        <v>0.13983050847457626</v>
+        <v>7.2033898305084734E-2</v>
       </c>
       <c r="Q7">
         <f t="shared" si="4"/>
@@ -2666,14 +2666,15 @@
         <v>2288.1355932203392</v>
       </c>
       <c r="K74">
-        <v>0.1059322033898305</v>
+        <f>E2/23.6</f>
+        <v>9.3220338983050849E-2</v>
       </c>
       <c r="L74">
         <v>0.26271186440677963</v>
       </c>
       <c r="M74">
         <f>10000*K74</f>
-        <v>1059.3220338983051</v>
+        <v>932.20338983050851</v>
       </c>
       <c r="N74">
         <f>10000*L74</f>
@@ -2724,14 +2725,15 @@
         <v>2669.4915254237285</v>
       </c>
       <c r="K75">
-        <v>0.11864406779661016</v>
+        <f>E3/23.6</f>
+        <v>0.1059322033898305</v>
       </c>
       <c r="L75">
         <v>0.26271186440677963</v>
       </c>
       <c r="M75">
         <f>10000*K75</f>
-        <v>1186.4406779661015</v>
+        <v>1059.3220338983051</v>
       </c>
       <c r="N75">
         <f>10000*L75</f>
@@ -2820,14 +2822,15 @@
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="K78">
-        <v>0.1271186440677966</v>
+        <f>E6/23.6</f>
+        <v>8.4745762711864403E-2</v>
       </c>
       <c r="L78">
         <v>0.26271186440677963</v>
       </c>
       <c r="M78">
         <f>10000*K78</f>
-        <v>1271.1864406779659</v>
+        <v>847.45762711864404</v>
       </c>
       <c r="N78">
         <f>10000*L78</f>
@@ -2856,14 +2859,15 @@
         <v>30</v>
       </c>
       <c r="K79">
-        <v>0.13983050847457626</v>
+        <f>E7/23.6</f>
+        <v>7.2033898305084734E-2</v>
       </c>
       <c r="L79">
         <v>0.26271186440677963</v>
       </c>
       <c r="M79">
         <f>10000*K79</f>
-        <v>1398.3050847457625</v>
+        <v>720.33898305084733</v>
       </c>
       <c r="N79">
         <f>10000*L79</f>

</xml_diff>